<commit_message>
Fix URL to template.
</commit_message>
<xml_diff>
--- a/lutra-cli/src/test/resources/eswc2019/instances/PizzaOntology-instances.xlsx
+++ b/lutra-cli/src/test/resources/eswc2019/instances/PizzaOntology-instances.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">template</t>
   </si>
   <si>
-    <t xml:space="preserve">https://tpl.ottr.xyz/pizza/0.1/NamedPizza.ttl</t>
+    <t xml:space="preserve">http://tpl.ottr.xyz/pizza/0.1/NamedPizza</t>
   </si>
   <si>
     <t xml:space="preserve">iri</t>
@@ -298,11 +298,11 @@
   </sheetPr>
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
@@ -556,9 +556,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" display="https://tpl.ottr.xyz/pizza/0.1/NamedPizza.ttl"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>